<commit_message>
ahora si estan bien los bac18,19y20
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-18-Catálogo de indicadores de logro.xlsx
+++ b/HT-6/Optica BAC-18-Catálogo de indicadores de logro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFCC5E7-C406-FF41-945E-F439C263D6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A16E260-A6E9-CC47-BA60-12DF6A19A240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Valor total de las ventas en el último año tomando en cuenta todos los productos y puntos de venta</t>
   </si>
   <si>
-    <t>Contento de trabajadores</t>
-  </si>
-  <si>
     <t>Porcentaje de clientes que vuelven a comprar en nuestra tienda teniendo en cuenta todo el historial de la tienda</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Porcentaje de aprobación de la óptica Vision por parte de los clientes en el mercado. Se obtiene mediante encuestas de satisfacción post venta</t>
+  </si>
+  <si>
+    <t>Rotación de trabajadores</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -630,10 +630,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.15">
@@ -641,10 +641,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.15">
@@ -652,10 +652,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.15">
@@ -663,10 +663,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.15">
@@ -674,10 +674,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.15">
@@ -685,32 +685,32 @@
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Optica BAC-18-Catálogo de indicadores de logro.xlsx
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-18-Catálogo de indicadores de logro.xlsx
+++ b/HT-6/Optica BAC-18-Catálogo de indicadores de logro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A16E260-A6E9-CC47-BA60-12DF6A19A240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9BFD1B-B0FB-D442-AB2C-CCDDAD088C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Descripción</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Rotación de trabajadores</t>
+  </si>
+  <si>
+    <t>OP-11</t>
+  </si>
+  <si>
+    <t>Ventas por internet</t>
+  </si>
+  <si>
+    <t>Número de ventas hechas mediante los canales digitales en el último año</t>
   </si>
 </sst>
 </file>
@@ -226,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -244,6 +253,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="133" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -713,6 +728,17 @@
         <v>33</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.15">
+      <c r="A16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adición de canales digitales (>
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-18-Catálogo de indicadores de logro.xlsx
+++ b/HT-6/Optica BAC-18-Catálogo de indicadores de logro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9BFD1B-B0FB-D442-AB2C-CCDDAD088C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB159F-1A32-594A-BD45-3546C215C91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -235,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,12 +253,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,13 +723,13 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>